<commit_message>
Correción, script y datos de BD
Se modificaron algunas propiedades en el modelo ER de la base de datos, también se agregó el script para crear la base de datos y un script para agregar datos de prueba a la base de datos.
</commit_message>
<xml_diff>
--- a/Base de datos/footballDEM_Normalizacion.xlsx
+++ b/Base de datos/footballDEM_Normalizacion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19890" windowHeight="8985" activeTab="4"/>
+    <workbookView windowWidth="19890" windowHeight="8535" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Modelo relacional" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111">
   <si>
     <t>TORNEO</t>
   </si>
@@ -345,6 +345,12 @@
   </si>
   <si>
     <t>ID_Alumno</t>
+  </si>
+  <si>
+    <t>SEMESTRE</t>
+  </si>
+  <si>
+    <t>NUA</t>
   </si>
 </sst>
 </file>
@@ -352,11 +358,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="h:mm\ AM/PM"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="h:mm\ AM/PM"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -384,21 +390,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -412,25 +403,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -450,6 +434,21 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -457,26 +456,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -488,9 +471,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -498,21 +487,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -527,10 +510,33 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -567,19 +573,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -591,37 +621,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -633,109 +633,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -748,6 +652,108 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -835,41 +841,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -901,8 +877,49 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -921,166 +938,155 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1093,14 +1099,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1122,27 +1120,18 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1158,7 +1147,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2033,160 +2022,160 @@
   </cols>
   <sheetData>
     <row r="2" ht="12" spans="2:6">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="F2" s="26" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" ht="12" spans="2:6">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" ht="12" spans="2:6">
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="8" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" ht="12" spans="4:6">
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" ht="12" spans="4:6">
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" ht="12" spans="4:6">
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" ht="12" spans="2:6">
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" ht="12" spans="2:6">
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="8" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" ht="12" spans="2:6">
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="8" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" ht="12" spans="2:6">
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="12" ht="12" spans="6:6">
-      <c r="F12" s="13" t="s">
+      <c r="F12" s="9" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="14" ht="12" spans="5:5">
-      <c r="E14" s="33" t="s">
+      <c r="E14" s="26" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="15" ht="12" spans="3:5">
-      <c r="C15" s="33" t="s">
+      <c r="C15" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="8" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="16" ht="12" spans="3:5">
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="8" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="17" ht="12" spans="3:5">
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="E17" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="18" ht="12" spans="3:5">
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="E18" s="8" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="19" ht="12" spans="3:5">
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="E19" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="20" ht="12" spans="3:5">
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E20" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="21" ht="12" spans="5:5">
-      <c r="E21" s="13" t="s">
+      <c r="E21" s="9" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2222,1118 +2211,1118 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
     </row>
     <row r="3" spans="2:12">
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
     </row>
     <row r="4" spans="2:12">
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
     </row>
     <row r="5" spans="2:12">
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
     </row>
     <row r="6" spans="2:12">
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
     </row>
     <row r="7" spans="2:12">
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="30"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
     </row>
     <row r="8" spans="2:12">
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="20">
+      <c r="C8" s="15">
         <v>1</v>
       </c>
-      <c r="D8" s="26">
+      <c r="D8" s="19">
         <v>43283</v>
       </c>
-      <c r="E8" s="26"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
     </row>
     <row r="9" spans="2:12">
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="20">
+      <c r="C9" s="15">
         <v>2</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
     </row>
     <row r="10" spans="2:12">
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="20">
+      <c r="C10" s="15">
         <v>3</v>
       </c>
-      <c r="D10" s="26" t="s">
+      <c r="D10" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
     </row>
     <row r="11" spans="2:12">
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="20">
+      <c r="C11" s="15">
         <v>4</v>
       </c>
-      <c r="D11" s="26" t="s">
+      <c r="D11" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
     </row>
     <row r="12" spans="2:12">
-      <c r="B12" s="35" t="s">
+      <c r="B12" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="20">
+      <c r="C12" s="15">
         <v>5</v>
       </c>
-      <c r="D12" s="26">
+      <c r="D12" s="19">
         <v>43284</v>
       </c>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
     </row>
     <row r="13" spans="2:12">
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="20">
+      <c r="C13" s="15">
         <v>6</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="20"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
     </row>
     <row r="14" spans="2:12">
-      <c r="B14" s="35" t="s">
+      <c r="B14" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="20">
+      <c r="C14" s="15">
         <v>7</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D14" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
     </row>
     <row r="15" spans="2:12">
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="20"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
     </row>
     <row r="16" spans="2:12">
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
-      <c r="L16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
     </row>
     <row r="17" spans="2:12">
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="21" t="s">
+      <c r="D17" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="21" t="s">
+      <c r="E17" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="21" t="s">
+      <c r="F17" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="G17" s="21" t="s">
+      <c r="G17" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="H17" s="22" t="s">
+      <c r="H17" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="J17" s="20"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="20"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
     </row>
     <row r="18" spans="2:12">
-      <c r="B18" s="35" t="s">
+      <c r="B18" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="20" t="s">
+      <c r="D18" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="E18" s="20" t="s">
+      <c r="E18" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="F18" s="31">
+      <c r="F18" s="24">
         <v>0.375</v>
       </c>
-      <c r="G18" s="20">
+      <c r="G18" s="15">
         <v>6</v>
       </c>
-      <c r="H18" s="20">
+      <c r="H18" s="15">
         <v>0</v>
       </c>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="20"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
     </row>
     <row r="19" spans="2:12">
-      <c r="B19" s="35" t="s">
+      <c r="B19" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="D19" s="20" t="s">
+      <c r="D19" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="E19" s="20" t="s">
+      <c r="E19" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="F19" s="31">
+      <c r="F19" s="24">
         <v>0.416666666666667</v>
       </c>
-      <c r="G19" s="20">
+      <c r="G19" s="15">
         <v>5</v>
       </c>
-      <c r="H19" s="20">
+      <c r="H19" s="15">
         <v>2</v>
       </c>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
     </row>
     <row r="20" spans="2:12">
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="D20" s="20" t="s">
+      <c r="D20" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="E20" s="20" t="s">
+      <c r="E20" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="F20" s="31">
+      <c r="F20" s="24">
         <v>0.458333333333333</v>
       </c>
-      <c r="G20" s="20">
+      <c r="G20" s="15">
         <v>1</v>
       </c>
-      <c r="H20" s="20">
+      <c r="H20" s="15">
         <v>5</v>
       </c>
-      <c r="J20" s="20"/>
-      <c r="K20" s="20"/>
-      <c r="L20" s="20"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
     </row>
     <row r="21" spans="2:12">
-      <c r="B21" s="35" t="s">
+      <c r="B21" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="D21" s="20" t="s">
+      <c r="D21" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="E21" s="20" t="s">
+      <c r="E21" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="F21" s="31">
+      <c r="F21" s="24">
         <v>0</v>
       </c>
-      <c r="G21" s="20">
+      <c r="G21" s="15">
         <v>6</v>
       </c>
-      <c r="H21" s="20">
+      <c r="H21" s="15">
         <v>5</v>
       </c>
-      <c r="J21" s="20"/>
-      <c r="K21" s="20"/>
-      <c r="L21" s="20"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
     </row>
     <row r="22" spans="2:12">
-      <c r="B22" s="20"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="20"/>
-      <c r="K22" s="20"/>
-      <c r="L22" s="20"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
     </row>
     <row r="23" spans="2:12">
-      <c r="B23" s="24" t="s">
+      <c r="B23" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="25"/>
-      <c r="K23" s="25"/>
-      <c r="L23" s="25"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
     </row>
     <row r="24" spans="2:12">
-      <c r="B24" s="21" t="s">
+      <c r="B24" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="21" t="s">
+      <c r="C24" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="21" t="s">
+      <c r="D24" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="21" t="s">
+      <c r="E24" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="F24" s="21" t="s">
+      <c r="F24" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="G24" s="21" t="s">
+      <c r="G24" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="H24" s="21" t="s">
+      <c r="H24" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="I24" s="21" t="s">
+      <c r="I24" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="J24" s="21" t="s">
+      <c r="J24" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="K24" s="21" t="s">
+      <c r="K24" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="L24" s="22" t="s">
+      <c r="L24" s="16" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="25" spans="2:12">
-      <c r="B25" s="35" t="s">
+      <c r="B25" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="28" t="s">
+      <c r="C25" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="D25" s="28" t="s">
+      <c r="D25" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="E25" s="28">
+      <c r="E25" s="21">
         <v>7</v>
       </c>
-      <c r="F25" s="20">
+      <c r="F25" s="15">
         <v>7</v>
       </c>
-      <c r="G25" s="20">
+      <c r="G25" s="15">
         <v>0</v>
       </c>
-      <c r="H25" s="20">
+      <c r="H25" s="15">
         <v>0</v>
       </c>
-      <c r="I25" s="20">
+      <c r="I25" s="15">
         <v>25</v>
       </c>
-      <c r="J25" s="20">
+      <c r="J25" s="15">
         <v>10</v>
       </c>
-      <c r="K25" s="20">
+      <c r="K25" s="15">
         <f>I25-J25</f>
         <v>15</v>
       </c>
-      <c r="L25" s="20">
+      <c r="L25" s="15">
         <f>F25*3+G25*1</f>
         <v>21</v>
       </c>
     </row>
     <row r="26" spans="2:12">
-      <c r="B26" s="35" t="s">
+      <c r="B26" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="C26" s="20" t="s">
+      <c r="C26" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="D26" s="20" t="s">
+      <c r="D26" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="E26" s="20">
+      <c r="E26" s="15">
         <v>7</v>
       </c>
-      <c r="F26" s="20">
+      <c r="F26" s="15">
         <v>6</v>
       </c>
-      <c r="G26" s="20">
+      <c r="G26" s="15">
         <v>1</v>
       </c>
-      <c r="H26" s="20">
+      <c r="H26" s="15">
         <v>0</v>
       </c>
-      <c r="I26" s="20">
+      <c r="I26" s="15">
         <v>27</v>
       </c>
-      <c r="J26" s="20">
+      <c r="J26" s="15">
         <v>13</v>
       </c>
-      <c r="K26" s="20">
+      <c r="K26" s="15">
         <f t="shared" ref="K26:K32" si="0">I26-J26</f>
         <v>14</v>
       </c>
-      <c r="L26" s="20">
+      <c r="L26" s="15">
         <f t="shared" ref="L26:L32" si="1">F26*3+G26*1</f>
         <v>19</v>
       </c>
     </row>
     <row r="27" spans="2:12">
-      <c r="B27" s="35" t="s">
+      <c r="B27" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="C27" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="D27" s="20" t="s">
+      <c r="D27" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="E27" s="20">
+      <c r="E27" s="15">
         <v>7</v>
       </c>
-      <c r="F27" s="20">
+      <c r="F27" s="15">
         <v>4</v>
       </c>
-      <c r="G27" s="20">
+      <c r="G27" s="15">
         <v>1</v>
       </c>
-      <c r="H27" s="20">
+      <c r="H27" s="15">
         <v>2</v>
       </c>
-      <c r="I27" s="20">
+      <c r="I27" s="15">
         <v>12</v>
       </c>
-      <c r="J27" s="20">
+      <c r="J27" s="15">
         <v>2</v>
       </c>
-      <c r="K27" s="20">
+      <c r="K27" s="15">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="L27" s="20">
+      <c r="L27" s="15">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
     </row>
     <row r="28" spans="2:12">
-      <c r="B28" s="35" t="s">
+      <c r="B28" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="C28" s="20" t="s">
+      <c r="C28" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="D28" s="20" t="s">
+      <c r="D28" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="E28" s="20">
+      <c r="E28" s="15">
         <v>7</v>
       </c>
-      <c r="F28" s="20">
+      <c r="F28" s="15">
         <v>4</v>
       </c>
-      <c r="G28" s="20">
+      <c r="G28" s="15">
         <v>0</v>
       </c>
-      <c r="H28" s="20">
+      <c r="H28" s="15">
         <v>3</v>
       </c>
-      <c r="I28" s="20">
+      <c r="I28" s="15">
         <v>3</v>
       </c>
-      <c r="J28" s="20">
+      <c r="J28" s="15">
         <v>12</v>
       </c>
-      <c r="K28" s="20">
+      <c r="K28" s="15">
         <f t="shared" si="0"/>
         <v>-9</v>
       </c>
-      <c r="L28" s="20">
+      <c r="L28" s="15">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
     </row>
     <row r="29" spans="2:12">
-      <c r="B29" s="35" t="s">
+      <c r="B29" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="C29" s="20" t="s">
+      <c r="C29" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="D29" s="20" t="s">
+      <c r="D29" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="E29" s="20">
+      <c r="E29" s="15">
         <v>7</v>
       </c>
-      <c r="F29" s="20">
+      <c r="F29" s="15">
         <v>2</v>
       </c>
-      <c r="G29" s="20">
+      <c r="G29" s="15">
         <v>0</v>
       </c>
-      <c r="H29" s="20">
+      <c r="H29" s="15">
         <v>5</v>
       </c>
-      <c r="I29" s="20">
+      <c r="I29" s="15">
         <v>8</v>
       </c>
-      <c r="J29" s="20">
+      <c r="J29" s="15">
         <v>14</v>
       </c>
-      <c r="K29" s="20">
+      <c r="K29" s="15">
         <f t="shared" si="0"/>
         <v>-6</v>
       </c>
-      <c r="L29" s="20">
+      <c r="L29" s="15">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
     </row>
     <row r="30" spans="2:12">
-      <c r="B30" s="35" t="s">
+      <c r="B30" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="C30" s="20" t="s">
+      <c r="C30" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="D30" s="20" t="s">
+      <c r="D30" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="E30" s="20">
+      <c r="E30" s="15">
         <v>7</v>
       </c>
-      <c r="F30" s="20">
+      <c r="F30" s="15">
         <v>1</v>
       </c>
-      <c r="G30" s="20">
+      <c r="G30" s="15">
         <v>0</v>
       </c>
-      <c r="H30" s="20">
+      <c r="H30" s="15">
         <v>6</v>
       </c>
-      <c r="I30" s="20">
+      <c r="I30" s="15">
         <v>5</v>
       </c>
-      <c r="J30" s="20">
+      <c r="J30" s="15">
         <v>11</v>
       </c>
-      <c r="K30" s="20">
+      <c r="K30" s="15">
         <f t="shared" si="0"/>
         <v>-6</v>
       </c>
-      <c r="L30" s="20">
+      <c r="L30" s="15">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
     <row r="31" spans="2:12">
-      <c r="B31" s="35" t="s">
+      <c r="B31" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="C31" s="20" t="s">
+      <c r="C31" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="D31" s="20" t="s">
+      <c r="D31" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="E31" s="20">
+      <c r="E31" s="15">
         <v>7</v>
       </c>
-      <c r="F31" s="20">
+      <c r="F31" s="15">
         <v>2</v>
       </c>
-      <c r="G31" s="20">
+      <c r="G31" s="15">
         <v>0</v>
       </c>
-      <c r="H31" s="20">
+      <c r="H31" s="15">
         <v>5</v>
       </c>
-      <c r="I31" s="20">
+      <c r="I31" s="15">
         <v>8</v>
       </c>
-      <c r="J31" s="20">
+      <c r="J31" s="15">
         <v>9</v>
       </c>
-      <c r="K31" s="20">
+      <c r="K31" s="15">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="L31" s="20">
+      <c r="L31" s="15">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
     </row>
     <row r="32" spans="2:12">
-      <c r="B32" s="35" t="s">
+      <c r="B32" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="C32" s="20" t="s">
+      <c r="C32" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D32" s="20" t="s">
+      <c r="D32" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="E32" s="20">
+      <c r="E32" s="15">
         <v>7</v>
       </c>
-      <c r="F32" s="20">
+      <c r="F32" s="15">
         <v>3</v>
       </c>
-      <c r="G32" s="20">
+      <c r="G32" s="15">
         <v>2</v>
       </c>
-      <c r="H32" s="20">
+      <c r="H32" s="15">
         <v>0</v>
       </c>
-      <c r="I32" s="20">
+      <c r="I32" s="15">
         <v>9</v>
       </c>
-      <c r="J32" s="20">
+      <c r="J32" s="15">
         <v>11</v>
       </c>
-      <c r="K32" s="20">
+      <c r="K32" s="15">
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-      <c r="L32" s="20">
+      <c r="L32" s="15">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
     </row>
     <row r="33" spans="2:12">
-      <c r="B33" s="20"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="20"/>
-      <c r="I33" s="20"/>
-      <c r="J33" s="20"/>
-      <c r="K33" s="20"/>
-      <c r="L33" s="20"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="15"/>
+      <c r="L33" s="15"/>
     </row>
     <row r="34" spans="2:12">
-      <c r="B34" s="27" t="s">
+      <c r="B34" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="32"/>
-      <c r="H34" s="20"/>
-      <c r="I34" s="20"/>
-      <c r="J34" s="20"/>
-      <c r="K34" s="20"/>
-      <c r="L34" s="20"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
+      <c r="K34" s="15"/>
+      <c r="L34" s="15"/>
     </row>
     <row r="35" spans="2:12">
-      <c r="B35" s="21" t="s">
+      <c r="B35" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C35" s="21" t="s">
+      <c r="C35" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D35" s="21" t="s">
+      <c r="D35" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="E35" s="21" t="s">
+      <c r="E35" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F35" s="22" t="s">
+      <c r="F35" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="H35" s="20"/>
-      <c r="I35" s="20"/>
-      <c r="J35" s="20"/>
-      <c r="K35" s="20"/>
-      <c r="L35" s="20"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="15"/>
+      <c r="L35" s="15"/>
     </row>
     <row r="36" spans="2:12">
-      <c r="B36" s="35" t="s">
+      <c r="B36" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C36" s="20" t="s">
+      <c r="C36" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="D36" s="20" t="s">
+      <c r="D36" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="E36" s="20">
+      <c r="E36" s="15">
         <v>28</v>
       </c>
-      <c r="F36" s="20" t="s">
+      <c r="F36" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="H36" s="20"/>
-      <c r="I36" s="20"/>
-      <c r="J36" s="20"/>
-      <c r="K36" s="20"/>
-      <c r="L36" s="20"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="15"/>
+      <c r="K36" s="15"/>
+      <c r="L36" s="15"/>
     </row>
     <row r="37" spans="2:12">
-      <c r="B37" s="35" t="s">
+      <c r="B37" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="C37" s="20" t="s">
+      <c r="C37" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="D37" s="20" t="s">
+      <c r="D37" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="E37" s="20">
+      <c r="E37" s="15">
         <v>26</v>
       </c>
-      <c r="F37" s="20" t="s">
+      <c r="F37" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="H37" s="20"/>
-      <c r="I37" s="20"/>
-      <c r="J37" s="20"/>
-      <c r="K37" s="20"/>
-      <c r="L37" s="20"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="15"/>
+      <c r="K37" s="15"/>
+      <c r="L37" s="15"/>
     </row>
     <row r="38" spans="2:12">
-      <c r="B38" s="20"/>
-      <c r="C38" s="20"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="20"/>
-      <c r="H38" s="20"/>
-      <c r="I38" s="20"/>
-      <c r="J38" s="20"/>
-      <c r="K38" s="20"/>
-      <c r="L38" s="20"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="15"/>
+      <c r="J38" s="15"/>
+      <c r="K38" s="15"/>
+      <c r="L38" s="15"/>
     </row>
     <row r="39" spans="2:12">
-      <c r="B39" s="27" t="s">
+      <c r="B39" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C39" s="27"/>
-      <c r="D39" s="27"/>
-      <c r="E39" s="27"/>
-      <c r="F39" s="27"/>
-      <c r="G39" s="27"/>
-      <c r="H39" s="27"/>
-      <c r="I39" s="32"/>
-      <c r="J39" s="20"/>
-      <c r="K39" s="20"/>
-      <c r="L39" s="20"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="25"/>
+      <c r="J39" s="15"/>
+      <c r="K39" s="15"/>
+      <c r="L39" s="15"/>
     </row>
     <row r="40" spans="2:12">
-      <c r="B40" s="21" t="s">
+      <c r="B40" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C40" s="21" t="s">
+      <c r="C40" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D40" s="21" t="s">
+      <c r="D40" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="E40" s="21" t="s">
+      <c r="E40" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F40" s="21" t="s">
+      <c r="F40" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="G40" s="21" t="s">
+      <c r="G40" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="H40" s="22" t="s">
+      <c r="H40" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="J40" s="20"/>
-      <c r="K40" s="20"/>
-      <c r="L40" s="20"/>
+      <c r="J40" s="15"/>
+      <c r="K40" s="15"/>
+      <c r="L40" s="15"/>
     </row>
     <row r="41" spans="2:12">
-      <c r="B41" s="35" t="s">
+      <c r="B41" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="20" t="s">
+      <c r="C41" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="D41" s="20" t="s">
+      <c r="D41" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="E41" s="20">
+      <c r="E41" s="15">
         <v>22</v>
       </c>
-      <c r="F41" s="20" t="s">
+      <c r="F41" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="G41" s="20" t="s">
+      <c r="G41" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="H41" s="20">
+      <c r="H41" s="15">
         <v>5</v>
       </c>
-      <c r="J41" s="20"/>
-      <c r="K41" s="20"/>
-      <c r="L41" s="20"/>
+      <c r="J41" s="15"/>
+      <c r="K41" s="15"/>
+      <c r="L41" s="15"/>
     </row>
     <row r="42" spans="2:12">
-      <c r="B42" s="35" t="s">
+      <c r="B42" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="C42" s="20" t="s">
+      <c r="C42" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="D42" s="20" t="s">
+      <c r="D42" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="E42" s="20">
+      <c r="E42" s="15">
         <v>22</v>
       </c>
-      <c r="F42" s="20" t="s">
+      <c r="F42" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="G42" s="20" t="s">
+      <c r="G42" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="H42" s="20">
+      <c r="H42" s="15">
         <v>1</v>
       </c>
-      <c r="J42" s="20"/>
-      <c r="K42" s="20"/>
-      <c r="L42" s="20"/>
+      <c r="J42" s="15"/>
+      <c r="K42" s="15"/>
+      <c r="L42" s="15"/>
     </row>
     <row r="43" spans="2:12">
-      <c r="B43" s="35" t="s">
+      <c r="B43" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="C43" s="20" t="s">
+      <c r="C43" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="D43" s="20" t="s">
+      <c r="D43" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="E43" s="20">
+      <c r="E43" s="15">
         <v>24</v>
       </c>
-      <c r="F43" s="20" t="s">
+      <c r="F43" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="G43" s="20" t="s">
+      <c r="G43" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="H43" s="20">
+      <c r="H43" s="15">
         <v>3</v>
       </c>
-      <c r="J43" s="20"/>
-      <c r="K43" s="20"/>
-      <c r="L43" s="20"/>
+      <c r="J43" s="15"/>
+      <c r="K43" s="15"/>
+      <c r="L43" s="15"/>
     </row>
     <row r="44" spans="2:12">
-      <c r="B44" s="35" t="s">
+      <c r="B44" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="C44" s="20" t="s">
+      <c r="C44" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="D44" s="20" t="s">
+      <c r="D44" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="E44" s="20">
+      <c r="E44" s="15">
         <v>25</v>
       </c>
-      <c r="F44" s="20" t="s">
+      <c r="F44" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="G44" s="20" t="s">
+      <c r="G44" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="H44" s="20">
+      <c r="H44" s="15">
         <v>2</v>
       </c>
-      <c r="J44" s="20"/>
-      <c r="K44" s="20"/>
-      <c r="L44" s="20"/>
+      <c r="J44" s="15"/>
+      <c r="K44" s="15"/>
+      <c r="L44" s="15"/>
     </row>
     <row r="45" spans="2:12">
-      <c r="B45" s="35" t="s">
+      <c r="B45" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="C45" s="20" t="s">
+      <c r="C45" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="D45" s="20" t="s">
+      <c r="D45" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="E45" s="20">
+      <c r="E45" s="15">
         <v>22</v>
       </c>
-      <c r="F45" s="20" t="s">
+      <c r="F45" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="G45" s="20" t="s">
+      <c r="G45" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="H45" s="20">
+      <c r="H45" s="15">
         <v>0</v>
       </c>
-      <c r="J45" s="20"/>
-      <c r="K45" s="20"/>
-      <c r="L45" s="20"/>
+      <c r="J45" s="15"/>
+      <c r="K45" s="15"/>
+      <c r="L45" s="15"/>
     </row>
     <row r="46" spans="2:8">
-      <c r="B46" s="35" t="s">
+      <c r="B46" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="C46" s="29" t="s">
+      <c r="C46" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="D46" s="29" t="s">
+      <c r="D46" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="E46" s="29">
+      <c r="E46" s="22">
         <v>24</v>
       </c>
-      <c r="F46" s="20" t="s">
+      <c r="F46" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="G46" s="29" t="s">
+      <c r="G46" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="H46" s="29">
+      <c r="H46" s="22">
         <v>5</v>
       </c>
     </row>
     <row r="47" spans="2:8">
-      <c r="B47" s="35" t="s">
+      <c r="B47" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="C47" s="29" t="s">
+      <c r="C47" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="D47" s="29" t="s">
+      <c r="D47" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="E47" s="29">
+      <c r="E47" s="22">
         <v>23</v>
       </c>
-      <c r="F47" s="20" t="s">
+      <c r="F47" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="G47" s="29" t="s">
+      <c r="G47" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="H47" s="29">
+      <c r="H47" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="2:8">
-      <c r="B48" s="35" t="s">
+      <c r="B48" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="C48" s="29" t="s">
+      <c r="C48" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="D48" s="29" t="s">
+      <c r="D48" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="E48" s="29">
+      <c r="E48" s="22">
         <v>22</v>
       </c>
-      <c r="F48" s="20" t="s">
+      <c r="F48" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="G48" s="29" t="s">
+      <c r="G48" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="H48" s="29">
+      <c r="H48" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="2:8">
-      <c r="B49" s="35" t="s">
+      <c r="B49" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="C49" s="28" t="s">
+      <c r="C49" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="D49" s="28" t="s">
+      <c r="D49" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="E49" s="28">
+      <c r="E49" s="21">
         <v>24</v>
       </c>
-      <c r="F49" s="28" t="s">
+      <c r="F49" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="G49" s="28" t="s">
+      <c r="G49" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="H49" s="28">
+      <c r="H49" s="21">
         <v>0</v>
       </c>
     </row>
@@ -3376,237 +3365,237 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="L2" s="7" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="3" spans="2:12">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="12" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="12" t="s">
+      <c r="E3" s="5"/>
+      <c r="F3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="9"/>
-      <c r="H3" s="14" t="s">
+      <c r="G3" s="5"/>
+      <c r="H3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="9"/>
-      <c r="J3" s="12" t="s">
+      <c r="I3" s="5"/>
+      <c r="J3" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="K3" s="9"/>
-      <c r="L3" s="12" t="s">
+      <c r="K3" s="5"/>
+      <c r="L3" s="8" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="2:12">
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="12" t="s">
+      <c r="C4" s="5"/>
+      <c r="D4" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="12" t="s">
+      <c r="E4" s="5"/>
+      <c r="F4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="15" t="s">
+      <c r="G4" s="5"/>
+      <c r="H4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="9"/>
-      <c r="J4" s="12" t="s">
+      <c r="I4" s="5"/>
+      <c r="J4" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="K4" s="9"/>
-      <c r="L4" s="12" t="s">
+      <c r="K4" s="5"/>
+      <c r="L4" s="8" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="2:12">
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="13" t="s">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="12" t="s">
+      <c r="E5" s="5"/>
+      <c r="F5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="15" t="s">
+      <c r="G5" s="5"/>
+      <c r="H5" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="9"/>
-      <c r="J5" s="12" t="s">
+      <c r="I5" s="5"/>
+      <c r="J5" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="K5" s="9"/>
-      <c r="L5" s="12" t="s">
+      <c r="K5" s="5"/>
+      <c r="L5" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="6" spans="2:12">
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="12" t="s">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="16" t="s">
+      <c r="G6" s="5"/>
+      <c r="H6" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="I6" s="9"/>
-      <c r="J6" s="12" t="s">
+      <c r="I6" s="5"/>
+      <c r="J6" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="K6" s="9"/>
-      <c r="L6" s="12" t="s">
+      <c r="K6" s="5"/>
+      <c r="L6" s="8" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="7" spans="2:12">
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="12" t="s">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="9"/>
-      <c r="H7" s="15" t="s">
+      <c r="G7" s="5"/>
+      <c r="H7" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="9"/>
-      <c r="J7" s="12" t="s">
+      <c r="I7" s="5"/>
+      <c r="J7" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="K7" s="9"/>
-      <c r="L7" s="13" t="s">
+      <c r="K7" s="5"/>
+      <c r="L7" s="9" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="8" spans="2:12">
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="12" t="s">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="9"/>
-      <c r="H8" s="15" t="s">
+      <c r="G8" s="5"/>
+      <c r="H8" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="9"/>
-      <c r="J8" s="12" t="s">
+      <c r="I8" s="5"/>
+      <c r="J8" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
     </row>
     <row r="9" spans="2:12">
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="13" t="s">
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="9"/>
-      <c r="H9" s="15" t="s">
+      <c r="G9" s="5"/>
+      <c r="H9" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="9"/>
-      <c r="J9" s="13" t="s">
+      <c r="I9" s="5"/>
+      <c r="J9" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
     </row>
     <row r="10" spans="2:12">
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="15" t="s">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
     </row>
     <row r="11" spans="2:12">
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="15" t="s">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
     </row>
     <row r="12" spans="2:12">
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="15" t="s">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
     </row>
     <row r="13" spans="2:12">
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="17" t="s">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -3655,7 +3644,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="2"/>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="1" t="s">
         <v>26</v>
       </c>
       <c r="K2" s="2"/>
@@ -3676,11 +3665,11 @@
         <v>7</v>
       </c>
       <c r="G3" s="4"/>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="I3" s="4"/>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="3" t="s">
         <v>28</v>
       </c>
       <c r="K3" s="4"/>
@@ -3689,7 +3678,7 @@
       </c>
     </row>
     <row r="4" spans="2:12">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="4"/>
@@ -3701,11 +3690,11 @@
         <v>9</v>
       </c>
       <c r="G4" s="4"/>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="I4" s="4"/>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="3" t="s">
         <v>34</v>
       </c>
       <c r="K4" s="4"/>
@@ -3714,7 +3703,7 @@
     <row r="5" spans="2:12">
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E5" s="4"/>
@@ -3722,11 +3711,11 @@
         <v>11</v>
       </c>
       <c r="G5" s="4"/>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I5" s="4"/>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="3" t="s">
         <v>35</v>
       </c>
       <c r="K5" s="4"/>
@@ -3741,7 +3730,7 @@
         <v>14</v>
       </c>
       <c r="G6" s="4"/>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="4" t="s">
         <v>106</v>
       </c>
       <c r="I6" s="4"/>
@@ -3758,15 +3747,15 @@
         <v>17</v>
       </c>
       <c r="G7" s="4"/>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="3" t="s">
         <v>10</v>
       </c>
       <c r="I7" s="4"/>
-      <c r="J7" s="10" t="s">
+      <c r="J7" s="6" t="s">
         <v>107</v>
       </c>
       <c r="K7" s="4"/>
-      <c r="L7" s="5"/>
+      <c r="L7" s="3"/>
     </row>
     <row r="8" spans="2:12">
       <c r="B8" s="4"/>
@@ -3777,11 +3766,11 @@
         <v>20</v>
       </c>
       <c r="G8" s="4"/>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="I8" s="4"/>
-      <c r="J8" s="9" t="s">
+      <c r="J8" s="5" t="s">
         <v>108</v>
       </c>
       <c r="K8" s="4"/>
@@ -3792,11 +3781,11 @@
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="3" t="s">
         <v>23</v>
       </c>
       <c r="G9" s="4"/>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="3" t="s">
         <v>15</v>
       </c>
       <c r="I9" s="4"/>
@@ -3813,7 +3802,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="3" t="s">
         <v>18</v>
       </c>
       <c r="I10" s="4"/>
@@ -3830,7 +3819,7 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="3" t="s">
         <v>21</v>
       </c>
       <c r="I11" s="4"/>
@@ -3847,7 +3836,7 @@
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="3" t="s">
         <v>24</v>
       </c>
       <c r="I12" s="4"/>
@@ -3864,7 +3853,7 @@
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="3" t="s">
         <v>25</v>
       </c>
       <c r="I13" s="4"/>
@@ -3896,12 +3885,13 @@
   <sheetPr/>
   <dimension ref="B2:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12"/>
   <cols>
+    <col min="1" max="1" width="2.19047619047619" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="3.71428571428571" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
@@ -3917,7 +3907,7 @@
   <sheetData>
     <row r="2" spans="2:12">
       <c r="B2" s="1" t="s">
-        <v>0</v>
+        <v>109</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
@@ -3932,7 +3922,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="2"/>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="1" t="s">
         <v>26</v>
       </c>
       <c r="K2" s="2"/>
@@ -3953,11 +3943,11 @@
         <v>7</v>
       </c>
       <c r="G3" s="4"/>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="I3" s="4"/>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="3" t="s">
         <v>28</v>
       </c>
       <c r="K3" s="4"/>
@@ -3966,47 +3956,49 @@
       </c>
     </row>
     <row r="4" spans="2:12">
-      <c r="B4" s="5" t="s">
-        <v>4</v>
+      <c r="B4" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="3" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E4" s="4"/>
-      <c r="F4" s="6" t="s">
-        <v>3</v>
+      <c r="F4" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I4" s="4"/>
-      <c r="J4" s="9" t="s">
+      <c r="J4" s="5" t="s">
         <v>108</v>
       </c>
       <c r="K4" s="4"/>
-      <c r="L4" s="9" t="s">
+      <c r="L4" s="5" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="5" spans="2:12">
-      <c r="B5" s="4"/>
+      <c r="B5" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="C5" s="4"/>
       <c r="D5" s="3" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="3" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="G5" s="4"/>
-      <c r="H5" s="6" t="s">
-        <v>28</v>
+      <c r="H5" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="I5" s="4"/>
-      <c r="J5" s="6" t="s">
-        <v>34</v>
+      <c r="J5" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="K5" s="4"/>
       <c r="L5" s="3"/>
@@ -4015,19 +4007,19 @@
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="3" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="G6" s="4"/>
-      <c r="H6" s="6" t="s">
-        <v>6</v>
+      <c r="H6" s="4" t="s">
+        <v>106</v>
       </c>
       <c r="I6" s="4"/>
-      <c r="J6" s="6" t="s">
-        <v>35</v>
+      <c r="J6" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="K6" s="4"/>
       <c r="L6" s="3"/>
@@ -4035,21 +4027,20 @@
     <row r="7" spans="2:12">
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
-      <c r="D7" s="5" t="s">
-        <v>22</v>
-      </c>
       <c r="E7" s="4"/>
       <c r="F7" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G7" s="4"/>
-      <c r="H7" s="6" t="s">
-        <v>8</v>
+      <c r="H7" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="I7" s="4"/>
-      <c r="J7" s="3"/>
+      <c r="J7" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="K7" s="4"/>
-      <c r="L7" s="5"/>
+      <c r="L7" s="3"/>
     </row>
     <row r="8" spans="2:12">
       <c r="B8" s="4"/>
@@ -4057,16 +4048,14 @@
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="3" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="G8" s="4"/>
-      <c r="H8" s="7" t="s">
-        <v>106</v>
+      <c r="H8" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="I8" s="4"/>
-      <c r="J8" s="10" t="s">
-        <v>107</v>
-      </c>
+      <c r="J8" s="3"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
     </row>
@@ -4076,15 +4065,15 @@
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G9" s="4"/>
-      <c r="H9" s="6" t="s">
-        <v>10</v>
+      <c r="H9" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="I9" s="4"/>
-      <c r="J9" s="9" t="s">
-        <v>108</v>
+      <c r="J9" s="6" t="s">
+        <v>107</v>
       </c>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
@@ -4095,15 +4084,15 @@
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G10" s="4"/>
-      <c r="H10" s="6" t="s">
-        <v>12</v>
+      <c r="H10" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="I10" s="4"/>
-      <c r="J10" s="4" t="s">
-        <v>30</v>
+      <c r="J10" s="5" t="s">
+        <v>108</v>
       </c>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
@@ -4113,16 +4102,13 @@
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
-      <c r="F11" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="G11" s="4"/>
-      <c r="H11" s="6" t="s">
-        <v>15</v>
+      <c r="H11" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="I11" s="4"/>
       <c r="J11" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
@@ -4132,14 +4118,13 @@
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
       <c r="G12" s="4"/>
-      <c r="H12" s="6" t="s">
-        <v>18</v>
+      <c r="H12" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
@@ -4151,12 +4136,12 @@
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
-      <c r="H13" s="6" t="s">
-        <v>21</v>
+      <c r="H13" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="I13" s="4"/>
-      <c r="J13" s="4" t="s">
-        <v>33</v>
+      <c r="J13" s="5" t="s">
+        <v>110</v>
       </c>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
@@ -4168,17 +4153,16 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="6" t="s">
-        <v>24</v>
-      </c>
       <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
+      <c r="J14" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="8:8">
-      <c r="H15" s="6" t="s">
-        <v>25</v>
+    <row r="15" spans="10:10">
+      <c r="J15" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>